<commit_message>
fix: uninitialized bug in http field parser bench code
</commit_message>
<xml_diff>
--- a/code/c/http-field-parser-bench/http-parser-bench.xlsx
+++ b/code/c/http-field-parser-bench/http-parser-bench.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>hs</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,10 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>548字节数据,100次循环,cycles数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>548字节数据,1000万次循环,cycles数(k)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -88,8 +84,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="179" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -134,13 +130,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -175,7 +171,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -315,7 +310,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -380,12 +374,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="240706768"/>
-        <c:axId val="42316256"/>
+        <c:axId val="178300176"/>
+        <c:axId val="178300736"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="240706768"/>
+        <c:axId val="178300176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -422,7 +416,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42316256"/>
+        <c:crossAx val="178300736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -430,7 +424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42316256"/>
+        <c:axId val="178300736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -481,7 +475,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240706768"/>
+        <c:crossAx val="178300176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -626,7 +620,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>特定字段提取!$B$2</c:f>
+              <c:f>特定字段提取!$B$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -706,7 +700,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>特定字段提取!$A$3:$A$7</c:f>
+              <c:f>特定字段提取!$A$32:$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -729,7 +723,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>特定字段提取!$B$3:$B$7</c:f>
+              <c:f>特定字段提取!$B$32:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -737,16 +731,16 @@
                   <c:v>4081992445</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3497801548</c:v>
+                  <c:v>3335864768</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2898859482</c:v>
+                  <c:v>2715290516</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>173302914</c:v>
+                  <c:v>2542863464</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>177617454</c:v>
+                  <c:v>677779298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -762,12 +756,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="816852000"/>
-        <c:axId val="238820368"/>
+        <c:axId val="178302976"/>
+        <c:axId val="178303536"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="816852000"/>
+        <c:axId val="178302976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,7 +798,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238820368"/>
+        <c:crossAx val="178303536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -812,7 +806,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238820368"/>
+        <c:axId val="178303536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,7 +857,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="816852000"/>
+        <c:crossAx val="178302976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1008,7 +1002,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>特定字段提取!$H$2</c:f>
+              <c:f>特定字段提取!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1088,7 +1082,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>特定字段提取!$G$3:$G$7</c:f>
+              <c:f>特定字段提取!$B$3:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1111,24 +1105,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>特定字段提取!$H$3:$H$7</c:f>
+              <c:f>特定字段提取!$C$3:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>56070</c:v>
+                  <c:v>40580</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>154758</c:v>
+                  <c:v>133653</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>135709</c:v>
+                  <c:v>126390</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2166</c:v>
+                  <c:v>88650</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2778</c:v>
+                  <c:v>11869</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1144,12 +1138,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="972751120"/>
-        <c:axId val="972753360"/>
+        <c:axId val="179003072"/>
+        <c:axId val="179003632"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="972751120"/>
+        <c:axId val="179003072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,7 +1180,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="972753360"/>
+        <c:crossAx val="179003632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1194,7 +1188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="972753360"/>
+        <c:axId val="179003632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,7 +1239,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="972751120"/>
+        <c:crossAx val="179003072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1386,393 +1380,11 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>特定字段提取!$B$33</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>548字节数据,100次循环,cycles数</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>特定字段提取!$A$34:$A$38</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>http-parser</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>hs</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>hs-lite</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>pico-hs</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>pico-avx2-hs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>特定字段提取!$B$34:$B$38</c:f>
-              <c:numCache>
-                <c:formatCode>0_);[Red]\(0\)</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>787825</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>512958</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>556224</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18588</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22717</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="755805648"/>
-        <c:axId val="755806208"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
-      <c:catAx>
-        <c:axId val="755805648"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="755806208"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="755806208"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0_);[Red]\(0\)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="755805648"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:depthPercent val="100"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:backWall>
-    <c:plotArea>
-      <c:layout/>
-      <c:bar3DChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>特定字段提取!$I$33</c:f>
+              <c:f>特定字段提取!$C$63</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1852,7 +1464,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>特定字段提取!$G$34:$G$38</c:f>
+              <c:f>特定字段提取!$A$64:$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1875,24 +1487,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>特定字段提取!$I$34:$I$38</c:f>
+              <c:f>特定字段提取!$C$64:$C$68</c:f>
               <c:numCache>
                 <c:formatCode>0_ </c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>34390572.314999998</c:v>
+                  <c:v>35407946.239</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22583956.449000001</c:v>
+                  <c:v>21423984.088</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22887476.254000001</c:v>
+                  <c:v>20478527.309</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1828140.345</c:v>
+                  <c:v>21480049.642999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1711613.702</c:v>
+                  <c:v>6673755.1859999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1908,8 +1520,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="984908896"/>
-        <c:axId val="982666992"/>
+        <c:axId val="179642400"/>
+        <c:axId val="179642960"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1922,7 +1534,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>特定字段提取!$H$33</c15:sqref>
+                          <c15:sqref>特定字段提取!$B$63</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1984,7 +1596,6 @@
                   <c:showLeaderLines val="0"/>
                   <c:extLst>
                     <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:layout/>
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
                         <c:spPr>
@@ -2008,7 +1619,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>特定字段提取!$G$34:$G$38</c15:sqref>
+                          <c15:sqref>特定字段提取!$A$64:$A$68</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2037,7 +1648,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>特定字段提取!$H$34:$H$38</c15:sqref>
+                          <c15:sqref>特定字段提取!$B$64:$B$68</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2045,19 +1656,19 @@
                       <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                       <c:ptCount val="5"/>
                       <c:pt idx="0">
-                        <c:v>34390572315</c:v>
+                        <c:v>35407946239</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>22583956449</c:v>
+                        <c:v>21423984088</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>22887476254</c:v>
+                        <c:v>20478527309</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1828140345</c:v>
+                        <c:v>21480049643</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>1711613702</c:v>
+                        <c:v>6673755186</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2068,7 +1679,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="984908896"/>
+        <c:axId val="179642400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2105,7 +1716,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="982666992"/>
+        <c:crossAx val="179642960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2113,7 +1724,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="982666992"/>
+        <c:axId val="179642960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2164,7 +1775,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="984908896"/>
+        <c:crossAx val="179642400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2373,46 +1984,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
@@ -3896,500 +3467,6 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4924,14 +4001,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4952,16 +4029,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4983,44 +4060,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="图表 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5034,7 +4081,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5356,202 +4403,313 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I39"/>
+  <dimension ref="A2:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
     <col min="7" max="7" width="13.75" customWidth="1"/>
     <col min="8" max="8" width="36.375" customWidth="1"/>
     <col min="9" max="9" width="36.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B2"/>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40580</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>133653</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>126390</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>88650</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>11869</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B10"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B16"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B18"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B20"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B21"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B23"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B24"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B25"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B26"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B27"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B28"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B32" s="1">
         <v>4081992445</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1">
+        <v>3335864768</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2715290516</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2542863464</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1">
+        <v>677779298</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B62"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <v>56070</v>
+      <c r="B64" s="1">
+        <v>35407946239</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="C64" s="3">
+        <f>B64/1000</f>
+        <v>35407946.239</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
-        <v>3497801548</v>
+      <c r="B65" s="1">
+        <v>21423984088</v>
       </c>
-      <c r="G4" t="s">
-        <v>0</v>
+      <c r="C65" s="3">
+        <f>B65/1000</f>
+        <v>21423984.088</v>
       </c>
-      <c r="H4" s="1">
-        <v>154758</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>2898859482</v>
+      <c r="B66" s="1">
+        <v>20478527309</v>
       </c>
-      <c r="G5" t="s">
-        <v>2</v>
+      <c r="C66" s="3">
+        <f t="shared" ref="C66:C68" si="0">B66/1000</f>
+        <v>20478527.309</v>
       </c>
-      <c r="H5" s="1">
-        <v>135709</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
-        <v>173302914</v>
+      <c r="B67" s="1">
+        <v>21480049643</v>
       </c>
-      <c r="G6" t="s">
-        <v>3</v>
+      <c r="C67" s="3">
+        <f t="shared" si="0"/>
+        <v>21480049.642999999</v>
       </c>
-      <c r="H6" s="1">
-        <v>2166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
-        <v>177617454</v>
+      <c r="B68" s="1">
+        <v>6673755186</v>
       </c>
-      <c r="G7" t="s">
-        <v>4</v>
+      <c r="C68" s="3">
+        <f t="shared" si="0"/>
+        <v>6673755.1859999998</v>
       </c>
-      <c r="H7" s="1">
-        <v>2778</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="1">
-        <v>787825</v>
-      </c>
-      <c r="G34" t="s">
-        <v>1</v>
-      </c>
-      <c r="H34" s="1">
-        <v>34390572315</v>
-      </c>
-      <c r="I34" s="3">
-        <f>H34/1000</f>
-        <v>34390572.314999998</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="1">
-        <v>512958</v>
-      </c>
-      <c r="G35" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1">
-        <v>22583956449</v>
-      </c>
-      <c r="I35" s="3">
-        <f>H35/1000</f>
-        <v>22583956.449000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="1">
-        <v>556224</v>
-      </c>
-      <c r="G36" t="s">
-        <v>2</v>
-      </c>
-      <c r="H36" s="1">
-        <v>22887476254</v>
-      </c>
-      <c r="I36" s="3">
-        <f t="shared" ref="I36:I38" si="0">H36/1000</f>
-        <v>22887476.254000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="1">
-        <v>18588</v>
-      </c>
-      <c r="G37" t="s">
-        <v>3</v>
-      </c>
-      <c r="H37" s="1">
-        <v>1828140345</v>
-      </c>
-      <c r="I37" s="3">
-        <f t="shared" si="0"/>
-        <v>1828140.345</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="1">
-        <v>22717</v>
-      </c>
-      <c r="G38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H38" s="1">
-        <v>1711613702</v>
-      </c>
-      <c r="I38" s="3">
-        <f t="shared" si="0"/>
-        <v>1711613.702</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H39" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B69"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B70"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B71"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B72"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B73"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B74"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B75"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B76"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B77"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B78"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B79"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B80"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B81"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B82"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B83"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B84"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B85"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B86"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B87"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B88"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B89"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B90"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fix: picohttpparser avx2 version and bench doc
</commit_message>
<xml_diff>
--- a/code/c/http-field-parser-bench/http-parser-bench.xlsx
+++ b/code/c/http-field-parser-bench/http-parser-bench.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>hs</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +76,10 @@
   </si>
   <si>
     <t>原始值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码错误不足信</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -374,12 +378,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="178300176"/>
-        <c:axId val="178300736"/>
+        <c:axId val="1602112"/>
+        <c:axId val="1602672"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="178300176"/>
+        <c:axId val="1602112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,7 +420,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178300736"/>
+        <c:crossAx val="1602672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -424,7 +428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="178300736"/>
+        <c:axId val="1602672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,7 +479,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178300176"/>
+        <c:crossAx val="1602112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -756,12 +760,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="178302976"/>
-        <c:axId val="178303536"/>
+        <c:axId val="1604912"/>
+        <c:axId val="1605472"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="178302976"/>
+        <c:axId val="1604912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,7 +802,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178303536"/>
+        <c:crossAx val="1605472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -806,7 +810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="178303536"/>
+        <c:axId val="1605472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -857,7 +861,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178302976"/>
+        <c:crossAx val="1604912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1138,12 +1142,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="179003072"/>
-        <c:axId val="179003632"/>
+        <c:axId val="1607712"/>
+        <c:axId val="1608272"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="179003072"/>
+        <c:axId val="1607712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,7 +1184,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179003632"/>
+        <c:crossAx val="1608272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1188,7 +1192,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179003632"/>
+        <c:axId val="1608272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,7 +1243,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179003072"/>
+        <c:crossAx val="1607712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1520,8 +1524,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="179642400"/>
-        <c:axId val="179642960"/>
+        <c:axId val="608437200"/>
+        <c:axId val="608437760"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1679,7 +1683,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="179642400"/>
+        <c:axId val="608437200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1716,7 +1720,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179642960"/>
+        <c:crossAx val="608437760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1724,7 +1728,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179642960"/>
+        <c:axId val="608437760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,7 +1779,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179642400"/>
+        <c:crossAx val="608437200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4000,13 +4004,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>342899</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:colOff>152401</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -4403,29 +4407,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C90"/>
+  <dimension ref="A2:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
     <col min="7" max="7" width="13.75" customWidth="1"/>
     <col min="8" max="8" width="36.375" customWidth="1"/>
     <col min="9" max="9" width="36.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B2"/>
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -4433,7 +4437,7 @@
         <v>40580</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -4441,7 +4445,7 @@
         <v>133653</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -4449,7 +4453,7 @@
         <v>126390</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4457,39 +4461,42 @@
         <v>88650</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>11869</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B8"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B9"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B10"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B11"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B12"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B13"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B14"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B15"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B16"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
@@ -4541,7 +4548,7 @@
         <v>4081992445</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -4549,7 +4556,7 @@
         <v>3335864768</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -4557,7 +4564,7 @@
         <v>2715290516</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -4565,12 +4572,15 @@
         <v>2542863464</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="1">
         <v>677779298</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
@@ -4596,7 +4606,7 @@
         <v>35407946.239</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -4608,7 +4618,7 @@
         <v>21423984.088</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -4620,7 +4630,7 @@
         <v>20478527.309</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -4632,7 +4642,7 @@
         <v>21480049.642999999</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -4643,42 +4653,45 @@
         <f t="shared" si="0"/>
         <v>6673755.1859999998</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D68" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B69"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B70"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B71"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B72"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B73"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B74"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B75"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B76"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B77"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B78"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B79"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B80"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.15">

</xml_diff>